<commit_message>
exclude integrity only tags
</commit_message>
<xml_diff>
--- a/Waterfall 3.0 to 3.1.xlsx
+++ b/Waterfall 3.0 to 3.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -1314,50 +1314,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1557,6 +1514,320 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>After!$A$5:$A$107</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>XX</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>N/A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>After!$M$5:$M$107</c:f>
@@ -1992,6 +2263,320 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>After!$A$5:$A$107</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>XX</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>N/A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>After!$N$5:$N$107</c:f>
@@ -2427,6 +3012,320 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>After!$A$5:$A$107</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>XX</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>N/A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>After!$O$5:$O$107</c:f>
@@ -2862,6 +3761,320 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>After!$A$5:$A$107</c:f>
+              <c:strCache>
+                <c:ptCount val="102"/>
+                <c:pt idx="0">
+                  <c:v>00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>XX</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>N/A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>After!$P$5:$P$107</c:f>
@@ -3275,6 +4488,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4108,7 +5322,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4303,7 +5517,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9295379" cy="6072187"/>
+    <xdr:ext cx="9311355" cy="6079977"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4346,6 +5560,7 @@
       <sheetName val="FCodeToUMCL+ToISOToFCode+"/>
       <sheetName val="MELDefaultCodeApplied"/>
       <sheetName val="Tables"/>
+      <sheetName val="WND Criticality - Rev 3"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -4358,6 +5573,7 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4381,6 +5597,7 @@
       <sheetName val="MELDefaultCodeApplied"/>
       <sheetName val="Tables"/>
       <sheetName val="AECriticalities"/>
+      <sheetName val="WND Criticality - Rev 3"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -4397,6 +5614,7 @@
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
+      <sheetData sheetId="14" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8089,7 +9307,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>

</xml_diff>